<commit_message>
feat: enable tensor calculus (resolve #57 and #2)
</commit_message>
<xml_diff>
--- a/instances/4node3pipe.xlsx
+++ b/instances/4node3pipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seunic-my.sharepoint.cn/personal/230208781_seu_edu_cn/Documents/★★★科研/Solverz/Solverz/instances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="11_AA477F009C7E9E0C495B15AE0F837397973A84AC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4B540A9-E227-48C2-AD39-B5B655F18954}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="11_AA477F009C7E9E0C495B15AE0F837397973A84AC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE120029-58B9-4285-87CA-91CB52E0E828}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,15 +23,15 @@
     <sheet name="Ts_set" sheetId="22" r:id="rId8"/>
     <sheet name="Tr_set" sheetId="23" r:id="rId9"/>
     <sheet name="phi_set" sheetId="24" r:id="rId10"/>
-    <sheet name="V" sheetId="27" r:id="rId11"/>
-    <sheet name="Node type" sheetId="28" r:id="rId12"/>
+    <sheet name="Pipe" sheetId="28" r:id="rId11"/>
+    <sheet name="Node" sheetId="29" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Ts</t>
   </si>
@@ -59,12 +59,24 @@
   <si>
     <t>phi</t>
   </si>
+  <si>
+    <t>f_node</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_node</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +96,13 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -121,9 +140,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -141,6 +163,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -431,7 +457,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A11"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -844,81 +870,232 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE14D37B-3CF5-4B7C-8071-4FE558846F33}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09890E01-8777-4BB5-A154-3AAC95634A49}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09890E01-8777-4BB5-A154-3AAC95634A49}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49BC84DB-7D8C-4D30-AC5D-41CC64B0F50D}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="1">
-        <v>0</v>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>